<commit_message>
Add model estimation for non-breast solids and taxanes
</commit_message>
<xml_diff>
--- a/appendixTableStudyCharacteristicsAndOutcomes.xlsx
+++ b/appendixTableStudyCharacteristicsAndOutcomes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="92">
   <si>
     <t>study</t>
   </si>
@@ -38,13 +38,19 @@
     <t>nITT</t>
   </si>
   <si>
+    <t>py</t>
+  </si>
+  <si>
     <t>nAMLOrMDS</t>
   </si>
   <si>
-    <t>py</t>
-  </si>
-  <si>
     <t>incidenceAMLOrMDS</t>
+  </si>
+  <si>
+    <t>nNonBreastSolid</t>
+  </si>
+  <si>
+    <t>incidenceNonBreastSolid</t>
   </si>
   <si>
     <t>Bergh (2000) SBG 9401</t>
@@ -366,17 +372,23 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="n">
         <v>38.0</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -385,25 +397,31 @@
         <v>251.0</v>
       </c>
       <c r="I2" t="n">
+        <v>801.1083333333332</v>
+      </c>
+      <c r="J2" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>801.1083333333332</v>
       </c>
       <c r="K2" t="n">
         <v>112.0</v>
       </c>
+      <c r="L2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>37.4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="n">
         <v>38.0</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" t="n">
         <v>180.0</v>
@@ -416,25 +434,31 @@
         <v>274.0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0</v>
+        <v>874.5166666666667</v>
       </c>
       <c r="J3" t="n">
-        <v>874.5166666666667</v>
+        <v>0.0</v>
       </c>
       <c r="K3" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>11.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="n">
         <v>73.0</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -443,25 +467,31 @@
         <v>255.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>1551.25</v>
       </c>
       <c r="J4" t="n">
-        <v>1551.25</v>
+        <v>0.0</v>
       </c>
       <c r="K4" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="n">
         <v>73.0</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E5" t="n">
         <v>480.0</v>
@@ -474,25 +504,31 @@
         <v>267.0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0</v>
+        <v>1624.25</v>
       </c>
       <c r="J5" t="n">
-        <v>1624.25</v>
+        <v>0.0</v>
       </c>
       <c r="K5" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>18.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="n">
         <v>73.0</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" t="n">
         <v>800.0</v>
@@ -505,25 +541,31 @@
         <v>255.0</v>
       </c>
       <c r="I6" t="n">
+        <v>1551.25</v>
+      </c>
+      <c r="J6" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1551.25</v>
       </c>
       <c r="K6" t="n">
         <v>19.3</v>
       </c>
+      <c r="L6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>38.7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="n">
         <v>110.0</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E7" t="n">
         <v>300.0</v>
@@ -536,25 +578,31 @@
         <v>289.0</v>
       </c>
       <c r="I7" t="n">
+        <v>2649.1666666666665</v>
+      </c>
+      <c r="J7" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>2649.1666666666665</v>
       </c>
       <c r="K7" t="n">
         <v>3.77</v>
       </c>
+      <c r="L7" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>34.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
         <v>110.0</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E8" t="n">
         <v>600.0</v>
@@ -567,25 +615,31 @@
         <v>276.0</v>
       </c>
       <c r="I8" t="n">
+        <v>2530.0</v>
+      </c>
+      <c r="J8" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2530.0</v>
       </c>
       <c r="K8" t="n">
         <v>3.95</v>
       </c>
+      <c r="L8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>47.4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="n">
         <v>36.0</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" t="n">
         <v>240.0</v>
@@ -600,25 +654,31 @@
         <v>484.0</v>
       </c>
       <c r="I9" t="n">
+        <v>1452.0</v>
+      </c>
+      <c r="J9" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1452.0</v>
       </c>
       <c r="K9" t="n">
         <v>13.8</v>
       </c>
+      <c r="L9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
         <v>36.0</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" t="n">
         <v>240.0</v>
@@ -633,25 +693,31 @@
         <v>493.0</v>
       </c>
       <c r="I10" t="n">
+        <v>1479.0</v>
+      </c>
+      <c r="J10" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1479.0</v>
       </c>
       <c r="K10" t="n">
         <v>20.3</v>
       </c>
+      <c r="L10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>67.6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
         <v>36.0</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" t="n">
         <v>240.0</v>
@@ -666,25 +732,31 @@
         <v>501.0</v>
       </c>
       <c r="I11" t="n">
+        <v>1503.0</v>
+      </c>
+      <c r="J11" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1503.0</v>
       </c>
       <c r="K11" t="n">
         <v>26.6</v>
       </c>
+      <c r="L11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>13.3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
         <v>36.0</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E12" t="n">
         <v>240.0</v>
@@ -699,25 +771,31 @@
         <v>495.0</v>
       </c>
       <c r="I12" t="n">
+        <v>1485.0</v>
+      </c>
+      <c r="J12" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1485.0</v>
       </c>
       <c r="K12" t="n">
         <v>13.5</v>
       </c>
+      <c r="L12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>67.3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="n">
         <v>100.0</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" t="n">
         <v>300.0</v>
@@ -729,22 +807,24 @@
       <c r="H13" t="n">
         <v>171.0</v>
       </c>
-      <c r="I13"/>
-      <c r="J13" t="n">
+      <c r="I13" t="n">
         <v>1419.2999999999997</v>
       </c>
+      <c r="J13"/>
       <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="n">
         <v>100.0</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E14" t="n">
         <v>600.0</v>
@@ -754,22 +834,24 @@
       <c r="H14" t="n">
         <v>173.0</v>
       </c>
-      <c r="I14"/>
-      <c r="J14" t="n">
+      <c r="I14" t="n">
         <v>1435.8999999999999</v>
       </c>
+      <c r="J14"/>
       <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="n">
         <v>58.0</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -777,22 +859,28 @@
       <c r="H15" t="n">
         <v>180.0</v>
       </c>
-      <c r="I15"/>
-      <c r="J15" t="n">
+      <c r="I15" t="n">
         <v>870.0</v>
       </c>
+      <c r="J15"/>
       <c r="K15"/>
+      <c r="L15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>46.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="n">
         <v>58.0</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -800,22 +888,24 @@
       <c r="H16" t="n">
         <v>199.0</v>
       </c>
-      <c r="I16"/>
-      <c r="J16" t="n">
+      <c r="I16" t="n">
         <v>961.8333333333333</v>
       </c>
+      <c r="J16"/>
       <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="n">
         <v>58.0</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E17" t="n">
         <v>400.0</v>
@@ -827,22 +917,28 @@
       <c r="H17" t="n">
         <v>180.0</v>
       </c>
-      <c r="I17"/>
-      <c r="J17" t="n">
+      <c r="I17" t="n">
         <v>870.0</v>
       </c>
+      <c r="J17"/>
       <c r="K17"/>
+      <c r="L17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>23.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="n">
         <v>58.0</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E18" t="n">
         <v>300.0</v>
@@ -854,22 +950,24 @@
       <c r="H18" t="n">
         <v>200.0</v>
       </c>
-      <c r="I18"/>
-      <c r="J18" t="n">
+      <c r="I18" t="n">
         <v>966.6666666666666</v>
       </c>
+      <c r="J18"/>
       <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19"/>
       <c r="C19" t="n">
         <v>84.0</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E19" t="n">
         <v>360.0</v>
@@ -884,25 +982,27 @@
         <v>545.0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0</v>
+        <v>3815.0</v>
       </c>
       <c r="J19" t="n">
-        <v>3815.0</v>
+        <v>0.0</v>
       </c>
       <c r="K19" t="n">
         <v>0.0</v>
       </c>
+      <c r="L19"/>
+      <c r="M19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="n">
         <v>84.0</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E20" t="n">
         <v>360.0</v>
@@ -917,25 +1017,27 @@
         <v>544.0</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0</v>
+        <v>3808.0</v>
       </c>
       <c r="J20" t="n">
-        <v>3808.0</v>
+        <v>0.0</v>
       </c>
       <c r="K20" t="n">
         <v>0.0</v>
       </c>
+      <c r="L20"/>
+      <c r="M20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="n">
         <v>84.0</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E21" t="n">
         <v>360.0</v>
@@ -950,25 +1052,27 @@
         <v>502.0</v>
       </c>
       <c r="I21" t="n">
+        <v>3514.0</v>
+      </c>
+      <c r="J21" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>3514.0</v>
       </c>
       <c r="K21" t="n">
         <v>5.69</v>
       </c>
+      <c r="L21"/>
+      <c r="M21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="n">
         <v>84.0</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E22" t="n">
         <v>360.0</v>
@@ -983,25 +1087,27 @@
         <v>500.0</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0</v>
+        <v>3500.0</v>
       </c>
       <c r="J22" t="n">
-        <v>3500.0</v>
+        <v>0.0</v>
       </c>
       <c r="K22" t="n">
         <v>0.0</v>
       </c>
+      <c r="L22"/>
+      <c r="M22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="n">
         <v>65.0</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E23" t="n">
         <v>240.0</v>
@@ -1016,25 +1122,27 @@
         <v>1649.0</v>
       </c>
       <c r="I23" t="n">
+        <v>8932.083333333334</v>
+      </c>
+      <c r="J23" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>8932.083333333334</v>
       </c>
       <c r="K23" t="n">
         <v>2.24</v>
       </c>
+      <c r="L23"/>
+      <c r="M23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="n">
         <v>65.0</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E24" t="n">
         <v>300.0</v>
@@ -1049,25 +1157,27 @@
         <v>1649.0</v>
       </c>
       <c r="I24" t="n">
+        <v>8932.083333333334</v>
+      </c>
+      <c r="J24" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>8932.083333333334</v>
       </c>
       <c r="K24" t="n">
         <v>4.48</v>
       </c>
+      <c r="L24"/>
+      <c r="M24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B25"/>
       <c r="C25" t="n">
         <v>72.0</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
@@ -1076,25 +1186,31 @@
         <v>164.0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0</v>
+        <v>984.0</v>
       </c>
       <c r="J25" t="n">
-        <v>984.0</v>
+        <v>0.0</v>
       </c>
       <c r="K25" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>30.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B26"/>
       <c r="C26" t="n">
         <v>72.0</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E26" t="n">
         <v>540.0</v>
@@ -1105,25 +1221,31 @@
         <v>174.0</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0</v>
+        <v>1044.0</v>
       </c>
       <c r="J26" t="n">
-        <v>1044.0</v>
+        <v>0.0</v>
       </c>
       <c r="K26" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>47.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B27"/>
       <c r="C27" t="n">
         <v>26.0</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E27" t="n">
         <v>240.0</v>
@@ -1135,22 +1257,24 @@
       <c r="H27" t="n">
         <v>734.0</v>
       </c>
-      <c r="I27"/>
-      <c r="J27" t="n">
+      <c r="I27" t="n">
         <v>1602.5666666666666</v>
       </c>
+      <c r="J27"/>
       <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B28"/>
       <c r="C28" t="n">
         <v>26.0</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E28" t="n">
         <v>240.0</v>
@@ -1162,22 +1286,24 @@
       <c r="H28" t="n">
         <v>728.0</v>
       </c>
-      <c r="I28"/>
-      <c r="J28" t="n">
+      <c r="I28" t="n">
         <v>1589.4666666666665</v>
       </c>
+      <c r="J28"/>
       <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B29"/>
       <c r="C29" t="n">
         <v>26.0</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
@@ -1185,22 +1311,24 @@
       <c r="H29" t="n">
         <v>732.0</v>
       </c>
-      <c r="I29"/>
-      <c r="J29" t="n">
+      <c r="I29" t="n">
         <v>1598.1999999999998</v>
       </c>
+      <c r="J29"/>
       <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="n">
         <v>69.0</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E30" t="n">
         <v>240.0</v>
@@ -1213,25 +1341,27 @@
         <v>767.0</v>
       </c>
       <c r="I30" t="n">
+        <v>4429.424999999999</v>
+      </c>
+      <c r="J30" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J30" t="n">
-        <v>4429.424999999999</v>
       </c>
       <c r="K30" t="n">
         <v>4.52</v>
       </c>
+      <c r="L30"/>
+      <c r="M30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B31"/>
       <c r="C31" t="n">
         <v>69.0</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E31" t="n">
         <v>240.0</v>
@@ -1244,25 +1374,27 @@
         <v>767.0</v>
       </c>
       <c r="I31" t="n">
+        <v>4429.424999999999</v>
+      </c>
+      <c r="J31" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J31" t="n">
-        <v>4429.424999999999</v>
       </c>
       <c r="K31" t="n">
         <v>2.26</v>
       </c>
+      <c r="L31"/>
+      <c r="M31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B32"/>
       <c r="C32" t="n">
         <v>69.0</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E32" t="n">
         <v>240.0</v>
@@ -1275,25 +1407,27 @@
         <v>772.0</v>
       </c>
       <c r="I32" t="n">
+        <v>4458.299999999999</v>
+      </c>
+      <c r="J32" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J32" t="n">
-        <v>4458.299999999999</v>
       </c>
       <c r="K32" t="n">
         <v>6.73</v>
       </c>
+      <c r="L32"/>
+      <c r="M32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B33"/>
       <c r="C33" t="n">
         <v>55.0</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E33" t="n">
         <v>240.0</v>
@@ -1306,25 +1440,27 @@
         <v>849.0</v>
       </c>
       <c r="I33" t="n">
+        <v>3905.4000000000005</v>
+      </c>
+      <c r="J33" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J33" t="n">
-        <v>3905.4000000000005</v>
       </c>
       <c r="K33" t="n">
         <v>10.2</v>
       </c>
+      <c r="L33"/>
+      <c r="M33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B34"/>
       <c r="C34" t="n">
         <v>55.0</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E34" t="n">
         <v>240.0</v>
@@ -1337,25 +1473,27 @@
         <v>847.0</v>
       </c>
       <c r="I34" t="n">
+        <v>3896.2000000000003</v>
+      </c>
+      <c r="J34" t="n">
         <v>10.0</v>
-      </c>
-      <c r="J34" t="n">
-        <v>3896.2000000000003</v>
       </c>
       <c r="K34" t="n">
         <v>25.7</v>
       </c>
+      <c r="L34"/>
+      <c r="M34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B35"/>
       <c r="C35" t="n">
         <v>55.0</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E35" t="n">
         <v>240.0</v>
@@ -1368,25 +1506,27 @@
         <v>849.0</v>
       </c>
       <c r="I35" t="n">
+        <v>3905.4000000000005</v>
+      </c>
+      <c r="J35" t="n">
         <v>8.0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>3905.4000000000005</v>
       </c>
       <c r="K35" t="n">
         <v>20.5</v>
       </c>
+      <c r="L35"/>
+      <c r="M35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B36"/>
       <c r="C36" t="n">
         <v>60.0</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>
@@ -1394,22 +1534,24 @@
       <c r="H36" t="n">
         <v>498.0</v>
       </c>
-      <c r="I36"/>
-      <c r="J36" t="n">
+      <c r="I36" t="n">
         <v>2490.0</v>
       </c>
+      <c r="J36"/>
       <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B37"/>
       <c r="C37" t="n">
         <v>60.0</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E37"/>
       <c r="F37"/>
@@ -1417,22 +1559,24 @@
       <c r="H37" t="n">
         <v>496.0</v>
       </c>
-      <c r="I37"/>
-      <c r="J37" t="n">
+      <c r="I37" t="n">
         <v>2480.0</v>
       </c>
+      <c r="J37"/>
       <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B38"/>
       <c r="C38" t="n">
         <v>60.0</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E38" t="n">
         <v>240.0</v>
@@ -1444,22 +1588,24 @@
       <c r="H38" t="n">
         <v>494.0</v>
       </c>
-      <c r="I38"/>
-      <c r="J38" t="n">
+      <c r="I38" t="n">
         <v>2470.0</v>
       </c>
+      <c r="J38"/>
       <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B39"/>
       <c r="C39" t="n">
         <v>60.0</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E39" t="n">
         <v>240.0</v>
@@ -1471,22 +1617,24 @@
       <c r="H39" t="n">
         <v>494.0</v>
       </c>
-      <c r="I39"/>
-      <c r="J39" t="n">
+      <c r="I39" t="n">
         <v>2470.0</v>
       </c>
+      <c r="J39"/>
       <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B40"/>
       <c r="C40" t="n">
         <v>62.0</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E40" t="n">
         <v>330.0</v>
@@ -1499,25 +1647,31 @@
         <v>297.0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0</v>
+        <v>1534.5</v>
       </c>
       <c r="J40" t="n">
-        <v>1534.5</v>
+        <v>0.0</v>
       </c>
       <c r="K40" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>19.6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B41"/>
       <c r="C41" t="n">
         <v>62.0</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E41" t="n">
         <v>440.0</v>
@@ -1528,25 +1682,31 @@
         <v>290.0</v>
       </c>
       <c r="I41" t="n">
+        <v>1498.3333333333335</v>
+      </c>
+      <c r="J41" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>1498.3333333333335</v>
       </c>
       <c r="K41" t="n">
         <v>6.67</v>
       </c>
+      <c r="L41" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>26.7</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B42"/>
       <c r="C42" t="n">
         <v>62.0</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E42" t="n">
         <v>300.0</v>
@@ -1556,22 +1716,24 @@
       <c r="H42" t="n">
         <v>481.0</v>
       </c>
-      <c r="I42"/>
-      <c r="J42" t="n">
+      <c r="I42" t="n">
         <v>2505.208333333333</v>
       </c>
+      <c r="J42"/>
       <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B43"/>
       <c r="C43" t="n">
         <v>62.0</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E43" t="n">
         <v>240.0</v>
@@ -1583,22 +1745,24 @@
       <c r="H43" t="n">
         <v>847.0</v>
       </c>
-      <c r="I43"/>
-      <c r="J43" t="n">
+      <c r="I43" t="n">
         <v>4411.458333333333</v>
       </c>
+      <c r="J43"/>
       <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B44"/>
       <c r="C44" t="n">
         <v>62.0</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E44" t="n">
         <v>225.0</v>
@@ -1610,22 +1774,24 @@
       <c r="H44" t="n">
         <v>960.0</v>
       </c>
-      <c r="I44"/>
-      <c r="J44" t="n">
+      <c r="I44" t="n">
         <v>5000.0</v>
       </c>
+      <c r="J44"/>
       <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B45"/>
       <c r="C45" t="n">
         <v>62.0</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E45" t="n">
         <v>200.0</v>
@@ -1637,22 +1803,24 @@
       <c r="H45" t="n">
         <v>959.0</v>
       </c>
-      <c r="I45"/>
-      <c r="J45" t="n">
+      <c r="I45" t="n">
         <v>4994.791666666666</v>
       </c>
+      <c r="J45"/>
       <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B46"/>
       <c r="C46" t="n">
         <v>131.0</v>
       </c>
       <c r="D46" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E46" t="n">
         <v>300.0</v>
@@ -1665,25 +1833,31 @@
         <v>212.0</v>
       </c>
       <c r="I46" t="n">
-        <v>0.0</v>
+        <v>2314.333333333333</v>
       </c>
       <c r="J46" t="n">
-        <v>2314.333333333333</v>
+        <v>0.0</v>
       </c>
       <c r="K46" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>21.6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B47"/>
       <c r="C47" t="n">
         <v>131.0</v>
       </c>
       <c r="D47" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E47" t="n">
         <v>150.0</v>
@@ -1696,25 +1870,31 @@
         <v>209.0</v>
       </c>
       <c r="I47" t="n">
+        <v>2281.583333333333</v>
+      </c>
+      <c r="J47" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J47" t="n">
-        <v>2281.583333333333</v>
       </c>
       <c r="K47" t="n">
         <v>8.77</v>
       </c>
+      <c r="L47" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>17.5</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B48"/>
       <c r="C48" t="n">
         <v>131.0</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E48" t="n">
         <v>225.0</v>
@@ -1727,25 +1907,31 @@
         <v>200.0</v>
       </c>
       <c r="I48" t="n">
+        <v>2183.333333333333</v>
+      </c>
+      <c r="J48" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J48" t="n">
-        <v>2183.333333333333</v>
       </c>
       <c r="K48" t="n">
         <v>4.58</v>
       </c>
+      <c r="L48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M48" t="n">
+        <v>9.16</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B49"/>
       <c r="C49" t="n">
         <v>80.0</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E49" t="n">
         <v>240.0</v>
@@ -1758,25 +1944,27 @@
         <v>1441.0</v>
       </c>
       <c r="I49" t="n">
+        <v>9546.625</v>
+      </c>
+      <c r="J49" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J49" t="n">
-        <v>9546.625</v>
       </c>
       <c r="K49" t="n">
         <v>7.33</v>
       </c>
+      <c r="L49"/>
+      <c r="M49"/>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B50"/>
       <c r="C50" t="n">
         <v>80.0</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E50" t="n">
         <v>240.0</v>
@@ -1789,25 +1977,27 @@
         <v>1441.0</v>
       </c>
       <c r="I50" t="n">
+        <v>9546.625</v>
+      </c>
+      <c r="J50" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>9546.625</v>
       </c>
       <c r="K50" t="n">
         <v>7.33</v>
       </c>
+      <c r="L50"/>
+      <c r="M50"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B51"/>
       <c r="C51" t="n">
         <v>69.0</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E51" t="n">
         <v>300.0</v>
@@ -1820,25 +2010,27 @@
         <v>1551.0</v>
       </c>
       <c r="I51" t="n">
+        <v>8918.25</v>
+      </c>
+      <c r="J51" t="n">
         <v>8.0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>8918.25</v>
       </c>
       <c r="K51" t="n">
         <v>8.97</v>
       </c>
+      <c r="L51"/>
+      <c r="M51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B52"/>
       <c r="C52" t="n">
         <v>69.0</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E52" t="n">
         <v>300.0</v>
@@ -1851,25 +2043,27 @@
         <v>1570.0</v>
       </c>
       <c r="I52" t="n">
+        <v>9027.5</v>
+      </c>
+      <c r="J52" t="n">
         <v>8.0</v>
-      </c>
-      <c r="J52" t="n">
-        <v>9027.5</v>
       </c>
       <c r="K52" t="n">
         <v>8.86</v>
       </c>
+      <c r="L52"/>
+      <c r="M52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B53"/>
       <c r="C53" t="n">
         <v>59.0</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E53" t="n">
         <v>225.0</v>
@@ -1883,22 +2077,24 @@
       <c r="H53" t="n">
         <v>751.0</v>
       </c>
-      <c r="I53"/>
-      <c r="J53" t="n">
+      <c r="I53" t="n">
         <v>3692.416666666667</v>
       </c>
+      <c r="J53"/>
       <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B54"/>
       <c r="C54" t="n">
         <v>59.0</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E54" t="n">
         <v>225.0</v>
@@ -1912,22 +2108,24 @@
       <c r="H54" t="n">
         <v>745.0</v>
       </c>
-      <c r="I54"/>
-      <c r="J54" t="n">
+      <c r="I54" t="n">
         <v>3662.916666666667</v>
       </c>
+      <c r="J54"/>
       <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B55"/>
       <c r="C55" t="n">
         <v>78.0</v>
       </c>
       <c r="D55" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E55" t="n">
         <v>600.0</v>
@@ -1940,25 +2138,27 @@
         <v>241.0</v>
       </c>
       <c r="I55" t="n">
+        <v>1566.5</v>
+      </c>
+      <c r="J55" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>1566.5</v>
       </c>
       <c r="K55" t="n">
         <v>6.38</v>
       </c>
+      <c r="L55"/>
+      <c r="M55"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B56"/>
       <c r="C56" t="n">
         <v>78.0</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E56" t="n">
         <v>300.0</v>
@@ -1969,25 +2169,27 @@
         <v>241.0</v>
       </c>
       <c r="I56" t="n">
-        <v>0.0</v>
+        <v>1566.5</v>
       </c>
       <c r="J56" t="n">
-        <v>1566.5</v>
+        <v>0.0</v>
       </c>
       <c r="K56" t="n">
         <v>0.0</v>
       </c>
+      <c r="L56"/>
+      <c r="M56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B57"/>
       <c r="C57" t="n">
         <v>86.0</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E57" t="n">
         <v>324.0</v>
@@ -2000,25 +2202,31 @@
         <v>1590.0</v>
       </c>
       <c r="I57" t="n">
+        <v>11448.0</v>
+      </c>
+      <c r="J57" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J57" t="n">
-        <v>11448.0</v>
       </c>
       <c r="K57" t="n">
         <v>11.4</v>
       </c>
+      <c r="L57" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>43.7</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B58"/>
       <c r="C58" t="n">
         <v>86.0</v>
       </c>
       <c r="D58" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E58" t="n">
         <v>324.0</v>
@@ -2031,25 +2239,31 @@
         <v>1524.0</v>
       </c>
       <c r="I58" t="n">
+        <v>10972.800000000001</v>
+      </c>
+      <c r="J58" t="n">
         <v>15.0</v>
-      </c>
-      <c r="J58" t="n">
-        <v>10972.800000000001</v>
       </c>
       <c r="K58" t="n">
         <v>13.7</v>
       </c>
+      <c r="L58" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>46.5</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B59"/>
       <c r="C59" t="n">
         <v>124.0</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E59" t="n">
         <v>300.0</v>
@@ -2064,25 +2278,27 @@
         <v>745.0</v>
       </c>
       <c r="I59" t="n">
+        <v>7698.333333333334</v>
+      </c>
+      <c r="J59" t="n">
         <v>6.0</v>
-      </c>
-      <c r="J59" t="n">
-        <v>7698.333333333334</v>
       </c>
       <c r="K59" t="n">
         <v>7.79</v>
       </c>
+      <c r="L59"/>
+      <c r="M59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B60"/>
       <c r="C60" t="n">
         <v>124.0</v>
       </c>
       <c r="D60" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E60" t="n">
         <v>300.0</v>
@@ -2095,25 +2311,27 @@
         <v>746.0</v>
       </c>
       <c r="I60" t="n">
+        <v>7708.666666666667</v>
+      </c>
+      <c r="J60" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J60" t="n">
-        <v>7708.666666666667</v>
       </c>
       <c r="K60" t="n">
         <v>2.59</v>
       </c>
+      <c r="L60"/>
+      <c r="M60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B61"/>
       <c r="C61" t="n">
         <v>65.0</v>
       </c>
       <c r="D61" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E61" t="n">
         <v>240.0</v>
@@ -2126,25 +2344,27 @@
         <v>1529.0</v>
       </c>
       <c r="I61" t="n">
+        <v>8282.083333333334</v>
+      </c>
+      <c r="J61" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J61" t="n">
-        <v>8282.083333333334</v>
       </c>
       <c r="K61" t="n">
         <v>2.41</v>
       </c>
+      <c r="L61"/>
+      <c r="M61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B62"/>
       <c r="C62" t="n">
         <v>65.0</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E62" t="n">
         <v>240.0</v>
@@ -2159,25 +2379,27 @@
         <v>1531.0</v>
       </c>
       <c r="I62" t="n">
+        <v>8292.916666666668</v>
+      </c>
+      <c r="J62" t="n">
         <v>6.0</v>
-      </c>
-      <c r="J62" t="n">
-        <v>8292.916666666668</v>
       </c>
       <c r="K62" t="n">
         <v>7.24</v>
       </c>
+      <c r="L62"/>
+      <c r="M62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B63"/>
       <c r="C63" t="n">
         <v>77.0</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E63" t="n">
         <v>300.0</v>
@@ -2192,25 +2414,31 @@
         <v>539.0</v>
       </c>
       <c r="I63" t="n">
-        <v>0.0</v>
+        <v>3458.5833333333335</v>
       </c>
       <c r="J63" t="n">
-        <v>3458.5833333333335</v>
+        <v>0.0</v>
       </c>
       <c r="K63" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L63" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M63" t="n">
+        <v>26.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B64"/>
       <c r="C64" t="n">
         <v>77.0</v>
       </c>
       <c r="D64" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E64" t="n">
         <v>300.0</v>
@@ -2223,25 +2451,31 @@
         <v>521.0</v>
       </c>
       <c r="I64" t="n">
-        <v>0.0</v>
+        <v>3343.0833333333335</v>
       </c>
       <c r="J64" t="n">
-        <v>3343.0833333333335</v>
+        <v>0.0</v>
       </c>
       <c r="K64" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L64" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="M64" t="n">
+        <v>47.9</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B65"/>
       <c r="C65" t="n">
         <v>63.0</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E65" t="n">
         <v>200.0</v>
@@ -2256,25 +2490,31 @@
         <v>951.0</v>
       </c>
       <c r="I65" t="n">
+        <v>5016.525</v>
+      </c>
+      <c r="J65" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J65" t="n">
-        <v>5016.525</v>
       </c>
       <c r="K65" t="n">
         <v>1.99</v>
       </c>
+      <c r="L65" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M65" t="n">
+        <v>17.9</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B66"/>
       <c r="C66" t="n">
         <v>63.0</v>
       </c>
       <c r="D66" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E66" t="n">
         <v>300.0</v>
@@ -2287,25 +2527,31 @@
         <v>974.0</v>
       </c>
       <c r="I66" t="n">
+        <v>5137.849999999999</v>
+      </c>
+      <c r="J66" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J66" t="n">
-        <v>5137.849999999999</v>
       </c>
       <c r="K66" t="n">
         <v>3.89</v>
       </c>
+      <c r="L66" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M66" t="n">
+        <v>19.5</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B67"/>
       <c r="C67" t="n">
         <v>191.0</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E67"/>
       <c r="F67"/>
@@ -2313,22 +2559,28 @@
       <c r="H67" t="n">
         <v>112.0</v>
       </c>
-      <c r="I67"/>
-      <c r="J67" t="n">
+      <c r="I67" t="n">
         <v>1780.8</v>
       </c>
+      <c r="J67"/>
       <c r="K67"/>
+      <c r="L67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>16.8</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B68"/>
       <c r="C68" t="n">
         <v>191.0</v>
       </c>
       <c r="D68" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E68" t="n">
         <v>360.0</v>
@@ -2340,22 +2592,28 @@
       <c r="H68" t="n">
         <v>137.0</v>
       </c>
-      <c r="I68"/>
-      <c r="J68" t="n">
+      <c r="I68" t="n">
         <v>2178.3</v>
       </c>
+      <c r="J68"/>
       <c r="K68"/>
+      <c r="L68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M68" t="n">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B69"/>
       <c r="C69" t="n">
         <v>70.0</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E69" t="n">
         <v>240.0</v>
@@ -2370,25 +2628,27 @@
         <v>271.0</v>
       </c>
       <c r="I69" t="n">
+        <v>1580.8333333333333</v>
+      </c>
+      <c r="J69" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J69" t="n">
-        <v>1580.8333333333333</v>
       </c>
       <c r="K69" t="n">
         <v>12.7</v>
       </c>
+      <c r="L69"/>
+      <c r="M69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B70"/>
       <c r="C70" t="n">
         <v>70.0</v>
       </c>
       <c r="D70" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E70" t="n">
         <v>320.0</v>
@@ -2401,25 +2661,27 @@
         <v>265.0</v>
       </c>
       <c r="I70" t="n">
+        <v>1545.8333333333333</v>
+      </c>
+      <c r="J70" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J70" t="n">
-        <v>1545.8333333333333</v>
       </c>
       <c r="K70" t="n">
         <v>19.4</v>
       </c>
+      <c r="L70"/>
+      <c r="M70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B71"/>
       <c r="C71" t="n">
         <v>59.0</v>
       </c>
       <c r="D71" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E71" t="n">
         <v>360.0</v>
@@ -2434,25 +2696,31 @@
         <v>978.0</v>
       </c>
       <c r="I71" t="n">
+        <v>4808.5</v>
+      </c>
+      <c r="J71" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J71" t="n">
-        <v>4808.5</v>
       </c>
       <c r="K71" t="n">
         <v>4.16</v>
       </c>
+      <c r="L71" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M71" t="n">
+        <v>18.7</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B72"/>
       <c r="C72" t="n">
         <v>59.0</v>
       </c>
       <c r="D72" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E72" t="n">
         <v>600.0</v>
@@ -2465,25 +2733,31 @@
         <v>795.0</v>
       </c>
       <c r="I72" t="n">
-        <v>0.0</v>
+        <v>3908.7500000000005</v>
       </c>
       <c r="J72" t="n">
-        <v>3908.7500000000005</v>
+        <v>0.0</v>
       </c>
       <c r="K72" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M72" t="n">
+        <v>10.2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B73"/>
       <c r="C73" t="n">
         <v>59.0</v>
       </c>
       <c r="D73" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E73"/>
       <c r="F73"/>
@@ -2492,23 +2766,29 @@
         <v>177.0</v>
       </c>
       <c r="I73" t="n">
-        <v>0.0</v>
+        <v>870.25</v>
       </c>
       <c r="J73" t="n">
-        <v>870.25</v>
+        <v>0.0</v>
       </c>
       <c r="K73" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M73" t="n">
+        <v>23.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E74"/>
       <c r="F74"/>
@@ -2517,15 +2797,17 @@
       <c r="I74"/>
       <c r="J74"/>
       <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E75"/>
       <c r="F75"/>
@@ -2534,15 +2816,17 @@
       <c r="I75"/>
       <c r="J75"/>
       <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E76"/>
       <c r="F76"/>
@@ -2551,17 +2835,19 @@
       <c r="I76"/>
       <c r="J76"/>
       <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B77"/>
       <c r="C77" t="n">
         <v>83.0</v>
       </c>
       <c r="D77" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E77"/>
       <c r="F77"/>
@@ -2570,25 +2856,31 @@
         <v>164.0</v>
       </c>
       <c r="I77" t="n">
-        <v>0.0</v>
+        <v>1134.3333333333335</v>
       </c>
       <c r="J77" t="n">
-        <v>1134.3333333333335</v>
+        <v>0.0</v>
       </c>
       <c r="K77" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L77" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M77" t="n">
+        <v>8.82</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B78"/>
       <c r="C78" t="n">
         <v>83.0</v>
       </c>
       <c r="D78" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E78" t="n">
         <v>300.0</v>
@@ -2601,25 +2893,31 @@
         <v>169.0</v>
       </c>
       <c r="I78" t="n">
+        <v>1168.9166666666667</v>
+      </c>
+      <c r="J78" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J78" t="n">
-        <v>1168.9166666666667</v>
       </c>
       <c r="K78" t="n">
         <v>8.55</v>
       </c>
+      <c r="L78" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M78" t="n">
+        <v>25.7</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B79"/>
       <c r="C79" t="n">
         <v>60.0</v>
       </c>
       <c r="D79" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E79" t="n">
         <v>600.0</v>
@@ -2632,25 +2930,27 @@
         <v>996.0</v>
       </c>
       <c r="I79" t="n">
+        <v>4980.0</v>
+      </c>
+      <c r="J79" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J79" t="n">
-        <v>4980.0</v>
       </c>
       <c r="K79" t="n">
         <v>6.02</v>
       </c>
+      <c r="L79"/>
+      <c r="M79"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B80"/>
       <c r="C80" t="n">
         <v>60.0</v>
       </c>
       <c r="D80" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E80" t="n">
         <v>300.0</v>
@@ -2665,25 +2965,27 @@
         <v>1003.0</v>
       </c>
       <c r="I80" t="n">
+        <v>5015.0</v>
+      </c>
+      <c r="J80" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J80" t="n">
-        <v>5015.0</v>
       </c>
       <c r="K80" t="n">
         <v>1.99</v>
       </c>
+      <c r="L80"/>
+      <c r="M80"/>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B81"/>
       <c r="C81" t="n">
         <v>29.0</v>
       </c>
       <c r="D81" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E81" t="n">
         <v>240.0</v>
@@ -2698,25 +3000,27 @@
         <v>872.0</v>
       </c>
       <c r="I81" t="n">
+        <v>2092.7999999999997</v>
+      </c>
+      <c r="J81" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J81" t="n">
-        <v>2092.7999999999997</v>
       </c>
       <c r="K81" t="n">
         <v>9.56</v>
       </c>
+      <c r="L81"/>
+      <c r="M81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B82"/>
       <c r="C82" t="n">
         <v>29.0</v>
       </c>
       <c r="D82" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E82" t="n">
         <v>240.0</v>
@@ -2731,25 +3035,27 @@
         <v>864.0</v>
       </c>
       <c r="I82" t="n">
+        <v>2073.6</v>
+      </c>
+      <c r="J82" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J82" t="n">
-        <v>2073.6</v>
       </c>
       <c r="K82" t="n">
         <v>4.82</v>
       </c>
+      <c r="L82"/>
+      <c r="M82"/>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B83"/>
       <c r="C83" t="n">
         <v>73.0</v>
       </c>
       <c r="D83" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E83" t="n">
         <v>240.0</v>
@@ -2762,25 +3068,27 @@
         <v>1142.0</v>
       </c>
       <c r="I83" t="n">
+        <v>6966.200000000001</v>
+      </c>
+      <c r="J83" t="n">
         <v>1.0</v>
-      </c>
-      <c r="J83" t="n">
-        <v>6966.200000000001</v>
       </c>
       <c r="K83" t="n">
         <v>1.44</v>
       </c>
+      <c r="L83"/>
+      <c r="M83"/>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B84"/>
       <c r="C84" t="n">
         <v>73.0</v>
       </c>
       <c r="D84" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E84" t="n">
         <v>360.0</v>
@@ -2793,25 +3101,27 @@
         <v>789.0</v>
       </c>
       <c r="I84" t="n">
+        <v>4812.900000000001</v>
+      </c>
+      <c r="J84" t="n">
         <v>5.0</v>
-      </c>
-      <c r="J84" t="n">
-        <v>4812.900000000001</v>
       </c>
       <c r="K84" t="n">
         <v>10.4</v>
       </c>
+      <c r="L84"/>
+      <c r="M84"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B85"/>
       <c r="C85" t="n">
         <v>73.0</v>
       </c>
       <c r="D85" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E85"/>
       <c r="F85"/>
@@ -2822,25 +3132,27 @@
         <v>1151.0</v>
       </c>
       <c r="I85" t="n">
-        <v>0.0</v>
+        <v>7021.1</v>
       </c>
       <c r="J85" t="n">
-        <v>7021.1</v>
+        <v>0.0</v>
       </c>
       <c r="K85" t="n">
         <v>0.0</v>
       </c>
+      <c r="L85"/>
+      <c r="M85"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B86"/>
       <c r="C86" t="n">
         <v>73.0</v>
       </c>
       <c r="D86" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E86"/>
       <c r="F86"/>
@@ -2851,25 +3163,27 @@
         <v>789.0</v>
       </c>
       <c r="I86" t="n">
-        <v>0.0</v>
+        <v>4812.900000000001</v>
       </c>
       <c r="J86" t="n">
-        <v>4812.900000000001</v>
+        <v>0.0</v>
       </c>
       <c r="K86" t="n">
         <v>0.0</v>
       </c>
+      <c r="L86"/>
+      <c r="M86"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B87"/>
       <c r="C87" t="n">
         <v>64.0</v>
       </c>
       <c r="D87" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E87" t="n">
         <v>300.0</v>
@@ -2884,25 +3198,27 @@
         <v>1630.0</v>
       </c>
       <c r="I87" t="n">
+        <v>8693.333333333332</v>
+      </c>
+      <c r="J87" t="n">
         <v>5.0</v>
-      </c>
-      <c r="J87" t="n">
-        <v>8693.333333333332</v>
       </c>
       <c r="K87" t="n">
         <v>5.75</v>
       </c>
+      <c r="L87"/>
+      <c r="M87"/>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B88"/>
       <c r="C88" t="n">
         <v>64.0</v>
       </c>
       <c r="D88" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E88" t="n">
         <v>240.0</v>
@@ -2917,25 +3233,27 @@
         <v>1634.0</v>
       </c>
       <c r="I88" t="n">
+        <v>8714.666666666666</v>
+      </c>
+      <c r="J88" t="n">
         <v>8.0</v>
-      </c>
-      <c r="J88" t="n">
-        <v>8714.666666666666</v>
       </c>
       <c r="K88" t="n">
         <v>9.18</v>
       </c>
+      <c r="L88"/>
+      <c r="M88"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B89"/>
       <c r="C89" t="n">
         <v>64.0</v>
       </c>
       <c r="D89" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E89" t="n">
         <v>240.0</v>
@@ -2950,25 +3268,27 @@
         <v>1630.0</v>
       </c>
       <c r="I89" t="n">
+        <v>8693.333333333332</v>
+      </c>
+      <c r="J89" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J89" t="n">
-        <v>8693.333333333332</v>
       </c>
       <c r="K89" t="n">
         <v>12.7</v>
       </c>
+      <c r="L89"/>
+      <c r="M89"/>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B90"/>
       <c r="C90" t="n">
         <v>125.0</v>
       </c>
       <c r="D90" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E90" t="n">
         <v>360.0</v>
@@ -2981,25 +3301,31 @@
         <v>604.0</v>
       </c>
       <c r="I90" t="n">
-        <v>0.0</v>
+        <v>6281.6</v>
       </c>
       <c r="J90" t="n">
-        <v>6281.6</v>
+        <v>0.0</v>
       </c>
       <c r="K90" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L90" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="M90" t="n">
+        <v>27.1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B91"/>
       <c r="C91" t="n">
         <v>125.0</v>
       </c>
       <c r="D91" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E91" t="n">
         <v>360.0</v>
@@ -3012,25 +3338,31 @@
         <v>610.0</v>
       </c>
       <c r="I91" t="n">
-        <v>0.0</v>
+        <v>6344.0</v>
       </c>
       <c r="J91" t="n">
-        <v>6344.0</v>
+        <v>0.0</v>
       </c>
       <c r="K91" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L91" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="M91" t="n">
+        <v>22.1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B92"/>
       <c r="C92" t="n">
         <v>64.0</v>
       </c>
       <c r="D92" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E92" t="n">
         <v>480.0</v>
@@ -3043,25 +3375,31 @@
         <v>360.0</v>
       </c>
       <c r="I92" t="n">
-        <v>0.0</v>
+        <v>1920.0</v>
       </c>
       <c r="J92" t="n">
-        <v>1920.0</v>
+        <v>0.0</v>
       </c>
       <c r="K92" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L92" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M92" t="n">
+        <v>20.8</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B93"/>
       <c r="C93" t="n">
         <v>64.0</v>
       </c>
       <c r="D93" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E93" t="n">
         <v>480.0</v>
@@ -3076,25 +3414,31 @@
         <v>368.0</v>
       </c>
       <c r="I93" t="n">
-        <v>0.0</v>
+        <v>1962.6666666666665</v>
       </c>
       <c r="J93" t="n">
-        <v>1962.6666666666665</v>
+        <v>0.0</v>
       </c>
       <c r="K93" t="n">
         <v>0.0</v>
+      </c>
+      <c r="L93" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M93" t="n">
+        <v>20.4</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B94"/>
       <c r="C94" t="n">
         <v>58.0</v>
       </c>
       <c r="D94" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E94" t="n">
         <v>600.0</v>
@@ -3105,25 +3449,31 @@
         <v>303.0</v>
       </c>
       <c r="I94" t="n">
+        <v>1454.3999999999999</v>
+      </c>
+      <c r="J94" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J94" t="n">
-        <v>1454.3999999999999</v>
       </c>
       <c r="K94" t="n">
         <v>13.8</v>
       </c>
+      <c r="L94" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M94" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B95"/>
       <c r="C95" t="n">
         <v>58.0</v>
       </c>
       <c r="D95" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E95"/>
       <c r="F95"/>
@@ -3132,25 +3482,31 @@
         <v>301.0</v>
       </c>
       <c r="I95" t="n">
-        <v>0.0</v>
+        <v>1444.8</v>
       </c>
       <c r="J95" t="n">
-        <v>1444.8</v>
+        <v>0.0</v>
       </c>
       <c r="K95" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M95" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B96"/>
       <c r="C96" t="n">
         <v>108.0</v>
       </c>
       <c r="D96" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E96" t="n">
         <v>240.0</v>
@@ -3162,22 +3518,24 @@
       <c r="H96" t="n">
         <v>751.0</v>
       </c>
-      <c r="I96"/>
-      <c r="J96" t="n">
+      <c r="I96" t="n">
         <v>6759.0</v>
       </c>
+      <c r="J96"/>
       <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B97"/>
       <c r="C97" t="n">
         <v>108.0</v>
       </c>
       <c r="D97" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E97" t="n">
         <v>240.0</v>
@@ -3189,11 +3547,13 @@
       <c r="H97" t="n">
         <v>742.0</v>
       </c>
-      <c r="I97"/>
-      <c r="J97" t="n">
+      <c r="I97" t="n">
         <v>6678.0</v>
       </c>
+      <c r="J97"/>
       <c r="K97"/>
+      <c r="L97"/>
+      <c r="M97"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Implement Meghan's data checks for non-breast solid malignancies
</commit_message>
<xml_diff>
--- a/appendixTableStudyCharacteristicsAndOutcomes.xlsx
+++ b/appendixTableStudyCharacteristicsAndOutcomes.xlsx
@@ -513,10 +513,10 @@
         <v>0.0</v>
       </c>
       <c r="L5" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="M5" t="n">
-        <v>18.5</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="6">
@@ -587,10 +587,10 @@
         <v>3.77</v>
       </c>
       <c r="L7" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="M7" t="n">
-        <v>34.0</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="8">
@@ -624,10 +624,10 @@
         <v>3.95</v>
       </c>
       <c r="L8" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="M8" t="n">
-        <v>47.4</v>
+        <v>59.3</v>
       </c>
     </row>
     <row r="9">
@@ -702,10 +702,10 @@
         <v>20.3</v>
       </c>
       <c r="L10" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="M10" t="n">
-        <v>67.6</v>
+        <v>74.4</v>
       </c>
     </row>
     <row r="11">
@@ -780,10 +780,10 @@
         <v>13.5</v>
       </c>
       <c r="L12" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="M12" t="n">
-        <v>67.3</v>
+        <v>74.1</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,9 @@
       <c r="E14" t="n">
         <v>600.0</v>
       </c>
-      <c r="F14"/>
+      <c r="F14" t="n">
+        <v>1800.0</v>
+      </c>
       <c r="G14"/>
       <c r="H14" t="n">
         <v>173.0</v>
@@ -1130,8 +1132,12 @@
       <c r="K23" t="n">
         <v>2.24</v>
       </c>
-      <c r="L23"/>
-      <c r="M23"/>
+      <c r="L23" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>38.1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -1165,8 +1171,12 @@
       <c r="K24" t="n">
         <v>4.48</v>
       </c>
-      <c r="L24"/>
-      <c r="M24"/>
+      <c r="L24" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>34.7</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -3008,8 +3018,12 @@
       <c r="K81" t="n">
         <v>9.56</v>
       </c>
-      <c r="L81"/>
-      <c r="M81"/>
+      <c r="L81" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="M81" t="n">
+        <v>62.1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
@@ -3043,8 +3057,12 @@
       <c r="K82" t="n">
         <v>4.82</v>
       </c>
-      <c r="L82"/>
-      <c r="M82"/>
+      <c r="L82" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M82" t="n">
+        <v>19.3</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s">

</xml_diff>

<commit_message>
Test the build on norm.ohsu.eud
</commit_message>
<xml_diff>
--- a/appendixTableStudyCharacteristicsAndOutcomes.xlsx
+++ b/appendixTableStudyCharacteristicsAndOutcomes.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>study</t>
   </si>
@@ -56,33 +56,81 @@
     <t>Bergh (2000) SBG 9401</t>
   </si>
   <si>
+    <t>FEC Tailored</t>
+  </si>
+  <si>
+    <t>FEC CTCb</t>
+  </si>
+  <si>
     <t>Bernard-Marty (2003)</t>
   </si>
   <si>
+    <t>CMF</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
     <t>Bonneterre (2005) FASG 05</t>
   </si>
   <si>
+    <t>FEC 50</t>
+  </si>
+  <si>
+    <t>FEC 100</t>
+  </si>
+  <si>
     <t>Citron (2003) Intergroup C9741</t>
   </si>
   <si>
+    <t>A-T-C</t>
+  </si>
+  <si>
+    <t>AC-T</t>
+  </si>
+  <si>
     <t>Colleoni (2009) IBCSG 15-95</t>
   </si>
   <si>
+    <t>AC-CMF</t>
+  </si>
+  <si>
     <t>Coombes (1996) ICCG 6-89/2-84</t>
   </si>
   <si>
+    <t>FEC</t>
+  </si>
+  <si>
     <t>Del Mastro (2015)</t>
   </si>
   <si>
+    <t>EC-T</t>
+  </si>
+  <si>
+    <t>FEC-T</t>
+  </si>
+  <si>
     <t>Eiermann (2011) BCIRG 005</t>
   </si>
   <si>
+    <t>TAC</t>
+  </si>
+  <si>
     <t>Fargeot (2004) FASG 08</t>
   </si>
   <si>
+    <t>Tamoxifen</t>
+  </si>
+  <si>
+    <t>EPI-Tam</t>
+  </si>
+  <si>
     <t>Fisher (1990) NSABP B-15</t>
   </si>
   <si>
+    <t>AC</t>
+  </si>
+  <si>
     <t>Fisher (1997) NSABP B-22</t>
   </si>
   <si>
@@ -92,33 +140,78 @@
     <t>Fisher (2001) NSABP B-23</t>
   </si>
   <si>
+    <t>CMF-Tam</t>
+  </si>
+  <si>
+    <t>AC-Tam</t>
+  </si>
+  <si>
     <t>Fountzilas (2005)</t>
   </si>
   <si>
+    <t>E-T-CMF</t>
+  </si>
+  <si>
+    <t>E-CMF</t>
+  </si>
+  <si>
     <t>Francis (2008) BIG 02-98</t>
   </si>
   <si>
+    <t>A-CMF</t>
+  </si>
+  <si>
+    <t>A-T-CMF</t>
+  </si>
+  <si>
+    <t>AT-CMF</t>
+  </si>
+  <si>
     <t>Fumoleu (2003) FASG 01</t>
   </si>
   <si>
+    <t>3 FEC 50</t>
+  </si>
+  <si>
+    <t>FEC 75</t>
+  </si>
+  <si>
     <t>Goldstein (2008) Intergroup E2197</t>
   </si>
   <si>
+    <t>AT</t>
+  </si>
+  <si>
     <t>Henderson (2003)</t>
   </si>
   <si>
     <t>Joensuu (2012) FinXX</t>
   </si>
   <si>
+    <t>TX-CEX</t>
+  </si>
+  <si>
+    <t>T-FEC</t>
+  </si>
+  <si>
     <t>Kerbrat (2007) FASG 09</t>
   </si>
   <si>
+    <t>E+Vnr</t>
+  </si>
+  <si>
     <t>Linden (2007) INT-0137</t>
   </si>
   <si>
+    <t>A-C</t>
+  </si>
+  <si>
     <t>Mackey (2013) BCIRG 001</t>
   </si>
   <si>
+    <t>FAC</t>
+  </si>
+  <si>
     <t>Mamounas (2005) NSABP B-28</t>
   </si>
   <si>
@@ -128,18 +221,33 @@
     <t>Martin (2013) GEICAM 2003-02</t>
   </si>
   <si>
+    <t>FAC-T</t>
+  </si>
+  <si>
     <t>Misset (1996)</t>
   </si>
   <si>
+    <t>AVCF</t>
+  </si>
+  <si>
     <t>Moore (2007) SWOG 9623</t>
   </si>
   <si>
+    <t>ACT</t>
+  </si>
+  <si>
     <t>Nitz (2014)</t>
   </si>
   <si>
     <t>Perez (2011) NCCTG N9831</t>
   </si>
   <si>
+    <t>AC-T+Trast</t>
+  </si>
+  <si>
+    <t>AC-T-Trast</t>
+  </si>
+  <si>
     <t>Roche (2006) FASG 06</t>
   </si>
   <si>
@@ -149,144 +257,34 @@
     <t>Romond (2005) NSABP B-31 &amp; N9831</t>
   </si>
   <si>
+    <t>ACT-T-Trast</t>
+  </si>
+  <si>
     <t>Shulman (2014) CALGB 40101</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>Swain (2013) NSABP B-38</t>
   </si>
   <si>
+    <t>AC-TG</t>
+  </si>
+  <si>
     <t>Venturini (2005)</t>
   </si>
   <si>
     <t>Vici (2012) GIOM 9902</t>
   </si>
   <si>
+    <t>T-EC</t>
+  </si>
+  <si>
     <t>Wils (1999) ICCG 4-87</t>
   </si>
   <si>
     <t>Wolmark (2001) NSABP B-18</t>
-  </si>
-  <si>
-    <t>FEC
-Tailored</t>
-  </si>
-  <si>
-    <t>FEC
-CTCb</t>
-  </si>
-  <si>
-    <t>CMF</t>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t>FEC 50</t>
-  </si>
-  <si>
-    <t>FEC 100</t>
-  </si>
-  <si>
-    <t>A-T-C</t>
-  </si>
-  <si>
-    <t>AC-T</t>
-  </si>
-  <si>
-    <t>AC-CMF</t>
-  </si>
-  <si>
-    <t>FEC</t>
-  </si>
-  <si>
-    <t>EC-T</t>
-  </si>
-  <si>
-    <t>FEC-T</t>
-  </si>
-  <si>
-    <t>TAC</t>
-  </si>
-  <si>
-    <t>Tamoxifen</t>
-  </si>
-  <si>
-    <t>EPI-Tam</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>CMF-Tam</t>
-  </si>
-  <si>
-    <t>AC-Tam</t>
-  </si>
-  <si>
-    <t>E-T-CMF</t>
-  </si>
-  <si>
-    <t>E-CMF</t>
-  </si>
-  <si>
-    <t>A-CMF</t>
-  </si>
-  <si>
-    <t>A-T-CMF</t>
-  </si>
-  <si>
-    <t>AT-CMF</t>
-  </si>
-  <si>
-    <t>3 FEC 50</t>
-  </si>
-  <si>
-    <t>FEC 75</t>
-  </si>
-  <si>
-    <t>AT</t>
-  </si>
-  <si>
-    <t>TX-CEX</t>
-  </si>
-  <si>
-    <t>T-FEC</t>
-  </si>
-  <si>
-    <t>E+Vnr</t>
-  </si>
-  <si>
-    <t>A-C</t>
-  </si>
-  <si>
-    <t>FAC</t>
-  </si>
-  <si>
-    <t>FAC-T</t>
-  </si>
-  <si>
-    <t>AVCF</t>
-  </si>
-  <si>
-    <t>ACT</t>
-  </si>
-  <si>
-    <t>AC-T+Trast</t>
-  </si>
-  <si>
-    <t>AC-T-Trast</t>
-  </si>
-  <si>
-    <t>ACT-T-Trast</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>AC-TG</t>
-  </si>
-  <si>
-    <t>T-EC</t>
   </si>
   <si>
     <t>Neo-AC</t>
@@ -295,12 +293,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11.0"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -311,7 +309,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -329,14 +327,295 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
@@ -387,32 +666,28 @@
       </c>
       <c r="B2"/>
       <c r="C2" t="n">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="n">
-        <v>675.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>8100.0</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2"/>
       <c r="H2" t="n">
-        <v>251.0</v>
+        <v> 251</v>
       </c>
       <c r="I2" t="n">
-        <v>801.1083333333332</v>
+        <v>801.108333333333</v>
       </c>
       <c r="J2" t="n">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="K2" t="n">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="L2" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M2" t="n">
         <v>37.4</v>
@@ -424,32 +699,32 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="n">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E3" t="n">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="F3" t="n">
-        <v>1200.0</v>
+        <v>1200</v>
       </c>
       <c r="G3"/>
       <c r="H3" t="n">
-        <v>274.0</v>
+        <v> 274</v>
       </c>
       <c r="I3" t="n">
-        <v>874.5166666666667</v>
+        <v>874.516666666667</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>11.4</v>
@@ -457,32 +732,32 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>255.0</v>
+        <v> 255</v>
       </c>
       <c r="I4" t="n">
         <v>1551.25</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M4" t="n">
         <v>25.8</v>
@@ -490,36 +765,36 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="F5" t="n">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="n">
-        <v>267.0</v>
+        <v> 267</v>
       </c>
       <c r="I5" t="n">
         <v>1624.25</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
         <v>24.6</v>
@@ -527,36 +802,36 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E6" t="n">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="F6" t="n">
-        <v>6640.0</v>
+        <v>6640</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="n">
-        <v>255.0</v>
+        <v> 255</v>
       </c>
       <c r="I6" t="n">
         <v>1551.25</v>
       </c>
       <c r="J6" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K6" t="n">
         <v>19.3</v>
       </c>
       <c r="L6" t="n">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="M6" t="n">
         <v>38.7</v>
@@ -564,36 +839,36 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="n">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F7" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>289.0</v>
+        <v> 289</v>
       </c>
       <c r="I7" t="n">
-        <v>2649.1666666666665</v>
+        <v>2649.16666666667</v>
       </c>
       <c r="J7" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>3.77</v>
       </c>
       <c r="L7" t="n">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="M7" t="n">
         <v>41.5</v>
@@ -601,36 +876,36 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="E8" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F8" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="n">
-        <v>276.0</v>
+        <v> 276</v>
       </c>
       <c r="I8" t="n">
-        <v>2530.0</v>
+        <v>2530</v>
       </c>
       <c r="J8" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
         <v>3.95</v>
       </c>
       <c r="L8" t="n">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="M8" t="n">
         <v>59.3</v>
@@ -638,38 +913,38 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="n">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E9" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F9" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G9" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H9" t="n">
-        <v>484.0</v>
+        <v> 484</v>
       </c>
       <c r="I9" t="n">
-        <v>1452.0</v>
+        <v>1452</v>
       </c>
       <c r="J9" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K9" t="n">
         <v>13.8</v>
       </c>
       <c r="L9" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
         <v>27.5</v>
@@ -677,38 +952,38 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E10" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F10" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G10" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H10" t="n">
-        <v>493.0</v>
+        <v> 493</v>
       </c>
       <c r="I10" t="n">
-        <v>1479.0</v>
+        <v>1479</v>
       </c>
       <c r="J10" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K10" t="n">
         <v>20.3</v>
       </c>
       <c r="L10" t="n">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="M10" t="n">
         <v>74.4</v>
@@ -716,38 +991,38 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E11" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F11" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G11" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H11" t="n">
-        <v>501.0</v>
+        <v> 501</v>
       </c>
       <c r="I11" t="n">
-        <v>1503.0</v>
+        <v>1503</v>
       </c>
       <c r="J11" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K11" t="n">
         <v>26.6</v>
       </c>
       <c r="L11" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M11" t="n">
         <v>13.3</v>
@@ -755,38 +1030,38 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E12" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F12" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G12" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H12" t="n">
-        <v>495.0</v>
+        <v> 495</v>
       </c>
       <c r="I12" t="n">
-        <v>1485.0</v>
+        <v>1485</v>
       </c>
       <c r="J12" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K12" t="n">
         <v>13.5</v>
       </c>
       <c r="L12" t="n">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="M12" t="n">
         <v>74.1</v>
@@ -794,27 +1069,27 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="n">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="E13" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F13" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>171.0</v>
+        <v> 171</v>
       </c>
       <c r="I13" t="n">
-        <v>1419.2999999999997</v>
+        <v>1419.3</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -823,27 +1098,27 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="n">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E14" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F14" t="n">
-        <v>1800.0</v>
+        <v>1800</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="n">
-        <v>173.0</v>
+        <v> 173</v>
       </c>
       <c r="I14" t="n">
-        <v>1435.8999999999999</v>
+        <v>1435.9</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
@@ -852,52 +1127,52 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="n">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15" t="n">
-        <v>180.0</v>
+        <v> 180</v>
       </c>
       <c r="I15" t="n">
-        <v>870.0</v>
+        <v>870</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
-        <v>46.0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="n">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16" t="n">
-        <v>199.0</v>
+        <v> 199</v>
       </c>
       <c r="I16" t="n">
-        <v>961.8333333333333</v>
+        <v>961.833333333333</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -906,60 +1181,60 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="n">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E17" t="n">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="F17" t="n">
-        <v>4800.0</v>
+        <v>4800</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="n">
-        <v>180.0</v>
+        <v> 180</v>
       </c>
       <c r="I17" t="n">
-        <v>870.0</v>
+        <v>870</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M17" t="n">
-        <v>23.0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="n">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E18" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F18" t="n">
-        <v>7200.0</v>
+        <v>7200</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="n">
-        <v>200.0</v>
+        <v> 200</v>
       </c>
       <c r="I18" t="n">
-        <v>966.6666666666666</v>
+        <v>966.666666666667</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
@@ -968,102 +1243,102 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B19"/>
       <c r="C19" t="n">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E19" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F19" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G19" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H19" t="n">
-        <v>545.0</v>
+        <v> 545</v>
       </c>
       <c r="I19" t="n">
-        <v>3815.0</v>
+        <v>3815</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L19"/>
       <c r="M19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="n">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E20" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F20" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G20" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H20" t="n">
-        <v>544.0</v>
+        <v> 544</v>
       </c>
       <c r="I20" t="n">
-        <v>3808.0</v>
+        <v>3808</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L20"/>
       <c r="M20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="n">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E21" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F21" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G21" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H21" t="n">
-        <v>502.0</v>
+        <v> 502</v>
       </c>
       <c r="I21" t="n">
-        <v>3514.0</v>
+        <v>3514</v>
       </c>
       <c r="J21" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K21" t="n">
         <v>5.69</v>
@@ -1073,73 +1348,73 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="n">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E22" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F22" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G22" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H22" t="n">
-        <v>500.0</v>
+        <v> 500</v>
       </c>
       <c r="I22" t="n">
-        <v>3500.0</v>
+        <v>3500</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L22"/>
       <c r="M22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="n">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E23" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F23" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G23" t="n">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="H23" t="n">
-        <v>1649.0</v>
+        <v>1649</v>
       </c>
       <c r="I23" t="n">
-        <v>8932.083333333334</v>
+        <v>8932.08333333333</v>
       </c>
       <c r="J23" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K23" t="n">
         <v>2.24</v>
       </c>
       <c r="L23" t="n">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="M23" t="n">
         <v>38.1</v>
@@ -1147,38 +1422,38 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="n">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="E24" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F24" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G24" t="n">
-        <v>450.0</v>
+        <v>450</v>
       </c>
       <c r="H24" t="n">
-        <v>1649.0</v>
+        <v>1649</v>
       </c>
       <c r="I24" t="n">
-        <v>8932.083333333334</v>
+        <v>8932.08333333333</v>
       </c>
       <c r="J24" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K24" t="n">
         <v>4.48</v>
       </c>
       <c r="L24" t="n">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="M24" t="n">
         <v>34.7</v>
@@ -1186,32 +1461,32 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B25"/>
       <c r="C25" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25" t="n">
-        <v>164.0</v>
+        <v> 164</v>
       </c>
       <c r="I25" t="n">
-        <v>984.0</v>
+        <v>984</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M25" t="n">
         <v>30.5</v>
@@ -1219,34 +1494,34 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B26"/>
       <c r="C26" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="E26" t="n">
-        <v>540.0</v>
+        <v>540</v>
       </c>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26" t="n">
-        <v>174.0</v>
+        <v> 174</v>
       </c>
       <c r="I26" t="n">
-        <v>1044.0</v>
+        <v>1044</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M26" t="n">
         <v>47.9</v>
@@ -1254,27 +1529,27 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B27"/>
       <c r="C27" t="n">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E27" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F27" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G27"/>
       <c r="H27" t="n">
-        <v>734.0</v>
+        <v> 734</v>
       </c>
       <c r="I27" t="n">
-        <v>1602.5666666666666</v>
+        <v>1602.56666666667</v>
       </c>
       <c r="J27"/>
       <c r="K27"/>
@@ -1283,27 +1558,27 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B28"/>
       <c r="C28" t="n">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="E28" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F28" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G28"/>
       <c r="H28" t="n">
-        <v>728.0</v>
+        <v> 728</v>
       </c>
       <c r="I28" t="n">
-        <v>1589.4666666666665</v>
+        <v>1589.46666666667</v>
       </c>
       <c r="J28"/>
       <c r="K28"/>
@@ -1312,23 +1587,23 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B29"/>
       <c r="C29" t="n">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29" t="n">
-        <v>732.0</v>
+        <v> 732</v>
       </c>
       <c r="I29" t="n">
-        <v>1598.1999999999998</v>
+        <v>1598.2</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
@@ -1337,30 +1612,30 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="n">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E30" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F30" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G30"/>
       <c r="H30" t="n">
-        <v>767.0</v>
+        <v> 767</v>
       </c>
       <c r="I30" t="n">
-        <v>4429.424999999999</v>
+        <v>4429.425</v>
       </c>
       <c r="J30" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K30" t="n">
         <v>4.52</v>
@@ -1370,30 +1645,30 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B31"/>
       <c r="C31" t="n">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E31" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F31" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G31"/>
       <c r="H31" t="n">
-        <v>767.0</v>
+        <v> 767</v>
       </c>
       <c r="I31" t="n">
-        <v>4429.424999999999</v>
+        <v>4429.425</v>
       </c>
       <c r="J31" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
         <v>2.26</v>
@@ -1403,30 +1678,30 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B32"/>
       <c r="C32" t="n">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E32" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F32" t="n">
-        <v>4800.0</v>
+        <v>4800</v>
       </c>
       <c r="G32"/>
       <c r="H32" t="n">
-        <v>772.0</v>
+        <v> 772</v>
       </c>
       <c r="I32" t="n">
-        <v>4458.299999999999</v>
+        <v>4458.3</v>
       </c>
       <c r="J32" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K32" t="n">
         <v>6.73</v>
@@ -1436,30 +1711,30 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B33"/>
       <c r="C33" t="n">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E33" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F33" t="n">
-        <v>4800.0</v>
+        <v>4800</v>
       </c>
       <c r="G33"/>
       <c r="H33" t="n">
-        <v>849.0</v>
+        <v> 849</v>
       </c>
       <c r="I33" t="n">
-        <v>3905.4000000000005</v>
+        <v>3905.4</v>
       </c>
       <c r="J33" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K33" t="n">
         <v>10.2</v>
@@ -1469,30 +1744,30 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B34"/>
       <c r="C34" t="n">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E34" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F34" t="n">
-        <v>4800.0</v>
+        <v>4800</v>
       </c>
       <c r="G34"/>
       <c r="H34" t="n">
-        <v>847.0</v>
+        <v> 847</v>
       </c>
       <c r="I34" t="n">
-        <v>3896.2000000000003</v>
+        <v>3896.2</v>
       </c>
       <c r="J34" t="n">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K34" t="n">
         <v>25.7</v>
@@ -1502,30 +1777,30 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B35"/>
       <c r="C35" t="n">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E35" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F35" t="n">
-        <v>9600.0</v>
+        <v>9600</v>
       </c>
       <c r="G35"/>
       <c r="H35" t="n">
-        <v>849.0</v>
+        <v> 849</v>
       </c>
       <c r="I35" t="n">
-        <v>3905.4000000000005</v>
+        <v>3905.4</v>
       </c>
       <c r="J35" t="n">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K35" t="n">
         <v>20.5</v>
@@ -1535,23 +1810,23 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B36"/>
       <c r="C36" t="n">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36"/>
       <c r="H36" t="n">
-        <v>498.0</v>
+        <v> 498</v>
       </c>
       <c r="I36" t="n">
-        <v>2490.0</v>
+        <v>2490</v>
       </c>
       <c r="J36"/>
       <c r="K36"/>
@@ -1560,23 +1835,23 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B37"/>
       <c r="C37" t="n">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
       <c r="H37" t="n">
-        <v>496.0</v>
+        <v> 496</v>
       </c>
       <c r="I37" t="n">
-        <v>2480.0</v>
+        <v>2480</v>
       </c>
       <c r="J37"/>
       <c r="K37"/>
@@ -1585,27 +1860,27 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B38"/>
       <c r="C38" t="n">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E38" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F38" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G38"/>
       <c r="H38" t="n">
-        <v>494.0</v>
+        <v> 494</v>
       </c>
       <c r="I38" t="n">
-        <v>2470.0</v>
+        <v>2470</v>
       </c>
       <c r="J38"/>
       <c r="K38"/>
@@ -1614,27 +1889,27 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B39"/>
       <c r="C39" t="n">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E39" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F39" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G39"/>
       <c r="H39" t="n">
-        <v>494.0</v>
+        <v> 494</v>
       </c>
       <c r="I39" t="n">
-        <v>2470.0</v>
+        <v>2470</v>
       </c>
       <c r="J39"/>
       <c r="K39"/>
@@ -1643,36 +1918,36 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B40"/>
       <c r="C40" t="n">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E40" t="n">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>750.0</v>
+        <v>750</v>
       </c>
       <c r="H40" t="n">
-        <v>297.0</v>
+        <v> 297</v>
       </c>
       <c r="I40" t="n">
         <v>1534.5</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M40" t="n">
         <v>19.6</v>
@@ -1680,34 +1955,34 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B41"/>
       <c r="C41" t="n">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E41" t="n">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41" t="n">
-        <v>290.0</v>
+        <v> 290</v>
       </c>
       <c r="I41" t="n">
-        <v>1498.3333333333335</v>
+        <v>1498.33333333333</v>
       </c>
       <c r="J41" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K41" t="n">
         <v>6.67</v>
       </c>
       <c r="L41" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M41" t="n">
         <v>26.7</v>
@@ -1715,25 +1990,25 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B42"/>
       <c r="C42" t="n">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D42" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="E42" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42" t="n">
-        <v>481.0</v>
+        <v> 481</v>
       </c>
       <c r="I42" t="n">
-        <v>2505.208333333333</v>
+        <v>2505.20833333333</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
@@ -1742,27 +2017,27 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B43"/>
       <c r="C43" t="n">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="E43" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F43" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G43"/>
       <c r="H43" t="n">
-        <v>847.0</v>
+        <v> 847</v>
       </c>
       <c r="I43" t="n">
-        <v>4411.458333333333</v>
+        <v>4411.45833333333</v>
       </c>
       <c r="J43"/>
       <c r="K43"/>
@@ -1771,27 +2046,27 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B44"/>
       <c r="C44" t="n">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="E44" t="n">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="H44" t="n">
-        <v>960.0</v>
+        <v> 960</v>
       </c>
       <c r="I44" t="n">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="J44"/>
       <c r="K44"/>
@@ -1800,27 +2075,27 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B45"/>
       <c r="C45" t="n">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="E45" t="n">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="H45" t="n">
-        <v>959.0</v>
+        <v> 959</v>
       </c>
       <c r="I45" t="n">
-        <v>4994.791666666666</v>
+        <v>4994.79166666667</v>
       </c>
       <c r="J45"/>
       <c r="K45"/>
@@ -1829,36 +2104,36 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B46"/>
       <c r="C46" t="n">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E46" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F46" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G46"/>
       <c r="H46" t="n">
-        <v>212.0</v>
+        <v> 212</v>
       </c>
       <c r="I46" t="n">
-        <v>2314.333333333333</v>
+        <v>2314.33333333333</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M46" t="n">
         <v>21.6</v>
@@ -1866,36 +2141,36 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B47"/>
       <c r="C47" t="n">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E47" t="n">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="F47" t="n">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="G47"/>
       <c r="H47" t="n">
-        <v>209.0</v>
+        <v> 209</v>
       </c>
       <c r="I47" t="n">
-        <v>2281.583333333333</v>
+        <v>2281.58333333333</v>
       </c>
       <c r="J47" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K47" t="n">
         <v>8.77</v>
       </c>
       <c r="L47" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M47" t="n">
         <v>17.5</v>
@@ -1903,36 +2178,36 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B48"/>
       <c r="C48" t="n">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="E48" t="n">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="F48" t="n">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="G48"/>
       <c r="H48" t="n">
-        <v>200.0</v>
+        <v> 200</v>
       </c>
       <c r="I48" t="n">
-        <v>2183.333333333333</v>
+        <v>2183.33333333333</v>
       </c>
       <c r="J48" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K48" t="n">
         <v>4.58</v>
       </c>
       <c r="L48" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M48" t="n">
         <v>9.16</v>
@@ -1940,30 +2215,30 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B49"/>
       <c r="C49" t="n">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E49" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H49" t="n">
-        <v>1441.0</v>
+        <v>1441</v>
       </c>
       <c r="I49" t="n">
         <v>9546.625</v>
       </c>
       <c r="J49" t="n">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K49" t="n">
         <v>7.33</v>
@@ -1973,30 +2248,30 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B50"/>
       <c r="C50" t="n">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E50" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F50" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G50"/>
       <c r="H50" t="n">
-        <v>1441.0</v>
+        <v>1441</v>
       </c>
       <c r="I50" t="n">
         <v>9546.625</v>
       </c>
       <c r="J50" t="n">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K50" t="n">
         <v>7.33</v>
@@ -2006,30 +2281,30 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B51"/>
       <c r="C51" t="n">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E51" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F51" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G51"/>
       <c r="H51" t="n">
-        <v>1551.0</v>
+        <v>1551</v>
       </c>
       <c r="I51" t="n">
         <v>8918.25</v>
       </c>
       <c r="J51" t="n">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K51" t="n">
         <v>8.97</v>
@@ -2039,30 +2314,30 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B52"/>
       <c r="C52" t="n">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E52" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F52" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G52"/>
       <c r="H52" t="n">
-        <v>1570.0</v>
+        <v>1570</v>
       </c>
       <c r="I52" t="n">
         <v>9027.5</v>
       </c>
       <c r="J52" t="n">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K52" t="n">
         <v>8.86</v>
@@ -2072,29 +2347,29 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B53"/>
       <c r="C53" t="n">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E53" t="n">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="F53" t="n">
-        <v>1800.0</v>
+        <v>1800</v>
       </c>
       <c r="G53" t="n">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="H53" t="n">
-        <v>751.0</v>
+        <v> 751</v>
       </c>
       <c r="I53" t="n">
-        <v>3692.416666666667</v>
+        <v>3692.41666666667</v>
       </c>
       <c r="J53"/>
       <c r="K53"/>
@@ -2103,29 +2378,29 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B54"/>
       <c r="C54" t="n">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E54" t="n">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="F54" t="n">
-        <v>1800.0</v>
+        <v>1800</v>
       </c>
       <c r="G54" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H54" t="n">
-        <v>745.0</v>
+        <v> 745</v>
       </c>
       <c r="I54" t="n">
-        <v>3662.916666666667</v>
+        <v>3662.91666666667</v>
       </c>
       <c r="J54"/>
       <c r="K54"/>
@@ -2134,30 +2409,30 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B55"/>
       <c r="C55" t="n">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E55" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F55" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G55"/>
       <c r="H55" t="n">
-        <v>241.0</v>
+        <v> 241</v>
       </c>
       <c r="I55" t="n">
         <v>1566.5</v>
       </c>
       <c r="J55" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K55" t="n">
         <v>6.38</v>
@@ -2167,67 +2442,67 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B56"/>
       <c r="C56" t="n">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="D56" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E56" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F56"/>
       <c r="G56"/>
       <c r="H56" t="n">
-        <v>241.0</v>
+        <v> 241</v>
       </c>
       <c r="I56" t="n">
         <v>1566.5</v>
       </c>
       <c r="J56" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L56"/>
       <c r="M56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B57"/>
       <c r="C57" t="n">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E57" t="n">
-        <v>324.0</v>
+        <v>324</v>
       </c>
       <c r="F57" t="n">
-        <v>7200.0</v>
+        <v>7200</v>
       </c>
       <c r="G57"/>
       <c r="H57" t="n">
-        <v>1590.0</v>
+        <v>1590</v>
       </c>
       <c r="I57" t="n">
-        <v>11448.0</v>
+        <v>11448</v>
       </c>
       <c r="J57" t="n">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="K57" t="n">
         <v>11.4</v>
       </c>
       <c r="L57" t="n">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M57" t="n">
         <v>43.7</v>
@@ -2235,36 +2510,36 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B58"/>
       <c r="C58" t="n">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="D58" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E58" t="n">
-        <v>324.0</v>
+        <v>324</v>
       </c>
       <c r="F58" t="n">
-        <v>7200.0</v>
+        <v>7200</v>
       </c>
       <c r="G58"/>
       <c r="H58" t="n">
-        <v>1524.0</v>
+        <v>1524</v>
       </c>
       <c r="I58" t="n">
-        <v>10972.800000000001</v>
+        <v>10972.8</v>
       </c>
       <c r="J58" t="n">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="K58" t="n">
         <v>13.7</v>
       </c>
       <c r="L58" t="n">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="M58" t="n">
         <v>46.5</v>
@@ -2272,32 +2547,32 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B59"/>
       <c r="C59" t="n">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="E59" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F59" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G59" t="n">
-        <v>450.0</v>
+        <v>450</v>
       </c>
       <c r="H59" t="n">
-        <v>745.0</v>
+        <v> 745</v>
       </c>
       <c r="I59" t="n">
-        <v>7698.333333333334</v>
+        <v>7698.33333333333</v>
       </c>
       <c r="J59" t="n">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K59" t="n">
         <v>7.79</v>
@@ -2307,30 +2582,30 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B60"/>
       <c r="C60" t="n">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E60" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F60" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G60"/>
       <c r="H60" t="n">
-        <v>746.0</v>
+        <v> 746</v>
       </c>
       <c r="I60" t="n">
-        <v>7708.666666666667</v>
+        <v>7708.66666666667</v>
       </c>
       <c r="J60" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K60" t="n">
         <v>2.59</v>
@@ -2340,30 +2615,30 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B61"/>
       <c r="C61" t="n">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E61" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F61" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G61"/>
       <c r="H61" t="n">
-        <v>1529.0</v>
+        <v>1529</v>
       </c>
       <c r="I61" t="n">
-        <v>8282.083333333334</v>
+        <v>8282.08333333333</v>
       </c>
       <c r="J61" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K61" t="n">
         <v>2.41</v>
@@ -2373,32 +2648,32 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B62"/>
       <c r="C62" t="n">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E62" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F62" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G62" t="n">
-        <v>900.0</v>
+        <v>900</v>
       </c>
       <c r="H62" t="n">
-        <v>1531.0</v>
+        <v>1531</v>
       </c>
       <c r="I62" t="n">
-        <v>8292.916666666668</v>
+        <v>8292.91666666667</v>
       </c>
       <c r="J62" t="n">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K62" t="n">
         <v>7.24</v>
@@ -2408,75 +2683,75 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B63"/>
       <c r="C63" t="n">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="D63" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="E63" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F63" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G63" t="n">
-        <v>450.0</v>
+        <v>450</v>
       </c>
       <c r="H63" t="n">
-        <v>539.0</v>
+        <v> 539</v>
       </c>
       <c r="I63" t="n">
-        <v>3458.5833333333335</v>
+        <v>3458.58333333333</v>
       </c>
       <c r="J63" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K63" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L63" t="n">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="M63" t="n">
-        <v>26.0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B64"/>
       <c r="C64" t="n">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E64" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F64" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G64"/>
       <c r="H64" t="n">
-        <v>521.0</v>
+        <v> 521</v>
       </c>
       <c r="I64" t="n">
-        <v>3343.0833333333335</v>
+        <v>3343.08333333333</v>
       </c>
       <c r="J64" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="M64" t="n">
         <v>47.9</v>
@@ -2484,38 +2759,38 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B65"/>
       <c r="C65" t="n">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E65" t="n">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="F65" t="n">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="G65" t="n">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="H65" t="n">
-        <v>951.0</v>
+        <v> 951</v>
       </c>
       <c r="I65" t="n">
         <v>5016.525</v>
       </c>
       <c r="J65" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K65" t="n">
         <v>1.99</v>
       </c>
       <c r="L65" t="n">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="M65" t="n">
         <v>17.9</v>
@@ -2523,36 +2798,36 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B66"/>
       <c r="C66" t="n">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E66" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F66" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G66"/>
       <c r="H66" t="n">
-        <v>974.0</v>
+        <v> 974</v>
       </c>
       <c r="I66" t="n">
-        <v>5137.849999999999</v>
+        <v>5137.85</v>
       </c>
       <c r="J66" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K66" t="n">
         <v>3.89</v>
       </c>
       <c r="L66" t="n">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M66" t="n">
         <v>19.5</v>
@@ -2560,20 +2835,20 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B67"/>
       <c r="C67" t="n">
-        <v>191.0</v>
+        <v>191</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E67"/>
       <c r="F67"/>
       <c r="G67"/>
       <c r="H67" t="n">
-        <v>112.0</v>
+        <v> 112</v>
       </c>
       <c r="I67" t="n">
         <v>1780.8</v>
@@ -2581,7 +2856,7 @@
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M67" t="n">
         <v>16.8</v>
@@ -2589,24 +2864,24 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B68"/>
       <c r="C68" t="n">
-        <v>191.0</v>
+        <v>191</v>
       </c>
       <c r="D68" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E68" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F68" t="n">
-        <v>14400.0</v>
+        <v>14400</v>
       </c>
       <c r="G68"/>
       <c r="H68" t="n">
-        <v>137.0</v>
+        <v> 137</v>
       </c>
       <c r="I68" t="n">
         <v>2178.3</v>
@@ -2614,7 +2889,7 @@
       <c r="J68"/>
       <c r="K68"/>
       <c r="L68" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M68" t="n">
         <v>13.8</v>
@@ -2622,32 +2897,32 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B69"/>
       <c r="C69" t="n">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E69" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F69" t="n">
-        <v>900.0</v>
+        <v>900</v>
       </c>
       <c r="G69" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="H69" t="n">
-        <v>271.0</v>
+        <v> 271</v>
       </c>
       <c r="I69" t="n">
-        <v>1580.8333333333333</v>
+        <v>1580.83333333333</v>
       </c>
       <c r="J69" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K69" t="n">
         <v>12.7</v>
@@ -2657,30 +2932,30 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B70"/>
       <c r="C70" t="n">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="D70" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E70" t="n">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="F70" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G70"/>
       <c r="H70" t="n">
-        <v>265.0</v>
+        <v> 265</v>
       </c>
       <c r="I70" t="n">
-        <v>1545.8333333333333</v>
+        <v>1545.83333333333</v>
       </c>
       <c r="J70" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K70" t="n">
         <v>19.4</v>
@@ -2690,38 +2965,38 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B71"/>
       <c r="C71" t="n">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E71" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F71" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G71" t="n">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="H71" t="n">
-        <v>978.0</v>
+        <v> 978</v>
       </c>
       <c r="I71" t="n">
         <v>4808.5</v>
       </c>
       <c r="J71" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K71" t="n">
         <v>4.16</v>
       </c>
       <c r="L71" t="n">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="M71" t="n">
         <v>18.7</v>
@@ -2729,36 +3004,36 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B72"/>
       <c r="C72" t="n">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="D72" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E72" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F72" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G72"/>
       <c r="H72" t="n">
-        <v>795.0</v>
+        <v> 795</v>
       </c>
       <c r="I72" t="n">
-        <v>3908.7500000000005</v>
+        <v>3908.75</v>
       </c>
       <c r="J72" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K72" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L72" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M72" t="n">
         <v>10.2</v>
@@ -2766,45 +3041,45 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B73"/>
       <c r="C73" t="n">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="D73" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E73"/>
       <c r="F73"/>
       <c r="G73"/>
       <c r="H73" t="n">
-        <v>177.0</v>
+        <v> 177</v>
       </c>
       <c r="I73" t="n">
         <v>870.25</v>
       </c>
       <c r="J73" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L73" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M73" t="n">
-        <v>23.0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E74"/>
       <c r="F74"/>
@@ -2818,12 +3093,12 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E75"/>
       <c r="F75"/>
@@ -2837,12 +3112,12 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E76"/>
       <c r="F76"/>
@@ -2856,32 +3131,32 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="B77"/>
       <c r="C77" t="n">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="D77" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E77"/>
       <c r="F77"/>
       <c r="G77"/>
       <c r="H77" t="n">
-        <v>164.0</v>
+        <v> 164</v>
       </c>
       <c r="I77" t="n">
-        <v>1134.3333333333335</v>
+        <v>1134.33333333333</v>
       </c>
       <c r="J77" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K77" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L77" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M77" t="n">
         <v>8.82</v>
@@ -2889,36 +3164,36 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="B78"/>
       <c r="C78" t="n">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E78" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F78" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G78"/>
       <c r="H78" t="n">
-        <v>169.0</v>
+        <v> 169</v>
       </c>
       <c r="I78" t="n">
-        <v>1168.9166666666667</v>
+        <v>1168.91666666667</v>
       </c>
       <c r="J78" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K78" t="n">
         <v>8.55</v>
       </c>
       <c r="L78" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M78" t="n">
         <v>25.7</v>
@@ -2926,30 +3201,30 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B79"/>
       <c r="C79" t="n">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D79" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E79" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F79" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G79"/>
       <c r="H79" t="n">
-        <v>996.0</v>
+        <v> 996</v>
       </c>
       <c r="I79" t="n">
-        <v>4980.0</v>
+        <v>4980</v>
       </c>
       <c r="J79" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K79" t="n">
         <v>6.02</v>
@@ -2959,32 +3234,32 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B80"/>
       <c r="C80" t="n">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D80" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E80" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F80" t="n">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="G80" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="H80" t="n">
-        <v>1003.0</v>
+        <v>1003</v>
       </c>
       <c r="I80" t="n">
-        <v>5015.0</v>
+        <v>5015</v>
       </c>
       <c r="J80" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K80" t="n">
         <v>1.99</v>
@@ -2994,38 +3269,38 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B81"/>
       <c r="C81" t="n">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="D81" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E81" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F81" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G81" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H81" t="n">
-        <v>872.0</v>
+        <v> 872</v>
       </c>
       <c r="I81" t="n">
-        <v>2092.7999999999997</v>
+        <v>2092.8</v>
       </c>
       <c r="J81" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K81" t="n">
         <v>9.56</v>
       </c>
       <c r="L81" t="n">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="M81" t="n">
         <v>62.1</v>
@@ -3033,38 +3308,38 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B82"/>
       <c r="C82" t="n">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="D82" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E82" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F82" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G82" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H82" t="n">
-        <v>864.0</v>
+        <v> 864</v>
       </c>
       <c r="I82" t="n">
         <v>2073.6</v>
       </c>
       <c r="J82" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K82" t="n">
         <v>4.82</v>
       </c>
       <c r="L82" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M82" t="n">
         <v>19.3</v>
@@ -3072,30 +3347,30 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B83"/>
       <c r="C83" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D83" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E83" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F83" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G83"/>
       <c r="H83" t="n">
-        <v>1142.0</v>
+        <v>1142</v>
       </c>
       <c r="I83" t="n">
-        <v>6966.200000000001</v>
+        <v>6966.2</v>
       </c>
       <c r="J83" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K83" t="n">
         <v>1.44</v>
@@ -3105,30 +3380,30 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B84"/>
       <c r="C84" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D84" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E84" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F84" t="n">
-        <v>3600.0</v>
+        <v>3600</v>
       </c>
       <c r="G84"/>
       <c r="H84" t="n">
-        <v>789.0</v>
+        <v> 789</v>
       </c>
       <c r="I84" t="n">
-        <v>4812.900000000001</v>
+        <v>4812.9</v>
       </c>
       <c r="J84" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K84" t="n">
         <v>10.4</v>
@@ -3138,94 +3413,94 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B85"/>
       <c r="C85" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D85" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E85"/>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="H85" t="n">
-        <v>1151.0</v>
+        <v>1151</v>
       </c>
       <c r="I85" t="n">
         <v>7021.1</v>
       </c>
       <c r="J85" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L85"/>
       <c r="M85"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B86"/>
       <c r="C86" t="n">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="D86" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E86"/>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="H86" t="n">
-        <v>789.0</v>
+        <v> 789</v>
       </c>
       <c r="I86" t="n">
-        <v>4812.900000000001</v>
+        <v>4812.9</v>
       </c>
       <c r="J86" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L86"/>
       <c r="M86"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B87"/>
       <c r="C87" t="n">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="D87" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E87" t="n">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F87" t="n">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="G87" t="n">
-        <v>450.0</v>
+        <v>450</v>
       </c>
       <c r="H87" t="n">
-        <v>1630.0</v>
+        <v>1630</v>
       </c>
       <c r="I87" t="n">
-        <v>8693.333333333332</v>
+        <v>8693.33333333333</v>
       </c>
       <c r="J87" t="n">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K87" t="n">
         <v>5.75</v>
@@ -3235,32 +3510,32 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B88"/>
       <c r="C88" t="n">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="D88" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E88" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F88" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G88" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H88" t="n">
-        <v>1634.0</v>
+        <v>1634</v>
       </c>
       <c r="I88" t="n">
-        <v>8714.666666666666</v>
+        <v>8714.66666666667</v>
       </c>
       <c r="J88" t="n">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K88" t="n">
         <v>9.18</v>
@@ -3270,32 +3545,32 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B89"/>
       <c r="C89" t="n">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="D89" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E89" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F89" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G89" t="n">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="H89" t="n">
-        <v>1630.0</v>
+        <v>1630</v>
       </c>
       <c r="I89" t="n">
-        <v>8693.333333333332</v>
+        <v>8693.33333333333</v>
       </c>
       <c r="J89" t="n">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K89" t="n">
         <v>12.7</v>
@@ -3305,36 +3580,36 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B90"/>
       <c r="C90" t="n">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="D90" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E90" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F90" t="n">
-        <v>3600.0</v>
+        <v>3600</v>
       </c>
       <c r="G90"/>
       <c r="H90" t="n">
-        <v>604.0</v>
+        <v> 604</v>
       </c>
       <c r="I90" t="n">
         <v>6281.6</v>
       </c>
       <c r="J90" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L90" t="n">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="M90" t="n">
         <v>27.1</v>
@@ -3342,36 +3617,36 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B91"/>
       <c r="C91" t="n">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="D91" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E91" t="n">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="F91" t="n">
-        <v>3600.0</v>
+        <v>3600</v>
       </c>
       <c r="G91"/>
       <c r="H91" t="n">
-        <v>610.0</v>
+        <v> 610</v>
       </c>
       <c r="I91" t="n">
-        <v>6344.0</v>
+        <v>6344</v>
       </c>
       <c r="J91" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K91" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L91" t="n">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="M91" t="n">
         <v>22.1</v>
@@ -3379,36 +3654,36 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="B92"/>
       <c r="C92" t="n">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="D92" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E92" t="n">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="F92" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G92"/>
       <c r="H92" t="n">
-        <v>360.0</v>
+        <v> 360</v>
       </c>
       <c r="I92" t="n">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="J92" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L92" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M92" t="n">
         <v>20.8</v>
@@ -3416,38 +3691,38 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="B93"/>
       <c r="C93" t="n">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="D93" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E93" t="n">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="F93" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G93" t="n">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="H93" t="n">
-        <v>368.0</v>
+        <v> 368</v>
       </c>
       <c r="I93" t="n">
-        <v>1962.6666666666665</v>
+        <v>1962.66666666667</v>
       </c>
       <c r="J93" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K93" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L93" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M93" t="n">
         <v>20.4</v>
@@ -3455,34 +3730,34 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B94"/>
       <c r="C94" t="n">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="D94" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="E94" t="n">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F94"/>
       <c r="G94"/>
       <c r="H94" t="n">
-        <v>303.0</v>
+        <v> 303</v>
       </c>
       <c r="I94" t="n">
-        <v>1454.3999999999999</v>
+        <v>1454.4</v>
       </c>
       <c r="J94" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K94" t="n">
         <v>13.8</v>
       </c>
       <c r="L94" t="n">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M94" t="n">
         <v>27.5</v>
@@ -3490,60 +3765,60 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B95"/>
       <c r="C95" t="n">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="D95" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E95"/>
       <c r="F95"/>
       <c r="G95"/>
       <c r="H95" t="n">
-        <v>301.0</v>
+        <v> 301</v>
       </c>
       <c r="I95" t="n">
         <v>1444.8</v>
       </c>
       <c r="J95" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K95" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L95" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M95" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B96"/>
       <c r="C96" t="n">
-        <v>108.0</v>
+        <v>108</v>
       </c>
       <c r="D96" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E96" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F96" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G96"/>
       <c r="H96" t="n">
-        <v>751.0</v>
+        <v> 751</v>
       </c>
       <c r="I96" t="n">
-        <v>6759.0</v>
+        <v>6759</v>
       </c>
       <c r="J96"/>
       <c r="K96"/>
@@ -3552,27 +3827,27 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B97"/>
       <c r="C97" t="n">
-        <v>108.0</v>
+        <v>108</v>
       </c>
       <c r="D97" t="s">
         <v>91</v>
       </c>
       <c r="E97" t="n">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="F97" t="n">
-        <v>2400.0</v>
+        <v>2400</v>
       </c>
       <c r="G97"/>
       <c r="H97" t="n">
-        <v>742.0</v>
+        <v> 742</v>
       </c>
       <c r="I97" t="n">
-        <v>6678.0</v>
+        <v>6678</v>
       </c>
       <c r="J97"/>
       <c r="K97"/>
@@ -3580,6 +3855,7 @@
       <c r="M97"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>